<commit_message>
Added Steps, Epics, Features, overall modification to allure reports
</commit_message>
<xml_diff>
--- a/nordson.omu/src/test/java/com/nordson/testData/PressureValues.xlsx
+++ b/nordson.omu/src/test/java/com/nordson/testData/PressureValues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi Raj\git\nordsonomu_automation\nordson.omu\src\test\java\com\nordson\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1E3994-9079-48C5-90B7-A33FA016581A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA8D65A-D6AF-406F-ABDE-0F994A140680}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="971" firstSheet="1" activeTab="1" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
   </bookViews>
   <sheets>
     <sheet name="kpaMinMaxSameValues" sheetId="1" r:id="rId1"/>
@@ -449,7 +449,7 @@
   <dimension ref="B1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C2"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,7 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF66B099-76A0-4630-B7C5-6712EE2C5428}">
   <dimension ref="B1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -728,7 +728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DACC4B9A-2110-4E2B-8390-C455D5AB778F}">
   <dimension ref="B1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>

</xml_diff>